<commit_message>
4 december, change absolute rel SE point, direction
</commit_message>
<xml_diff>
--- a/bsp2/AllTogether.xlsx
+++ b/bsp2/AllTogether.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmsil\Desktop\Desktop\School\S3\bsp3\bsp2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmsil\Desktop\bsp3\bsp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFCE412-308C-4EFC-855F-0DFDB2A1D580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D347F9F3-1AF5-4B78-986C-DE827952989D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9105" yWindow="4440" windowWidth="28800" windowHeight="15345" xr2:uid="{7E49008B-DF2A-43E1-A042-1C73C57D9710}"/>
+    <workbookView minimized="1" xWindow="9705" yWindow="5085" windowWidth="25875" windowHeight="15345" xr2:uid="{79F8FA3C-B5BD-4925-A4D7-8184B102EEA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Wall" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="191">
   <si>
     <t>StairsID</t>
   </si>
@@ -115,6 +115,27 @@
     <t>VectorY</t>
   </si>
   <si>
+    <t>VectorX</t>
+  </si>
+  <si>
+    <t>EndPointx</t>
+  </si>
+  <si>
+    <t>EndPointz</t>
+  </si>
+  <si>
+    <t>EndPointy</t>
+  </si>
+  <si>
+    <t>StartPointz</t>
+  </si>
+  <si>
+    <t>StartPointy</t>
+  </si>
+  <si>
+    <t>StartPointx</t>
+  </si>
+  <si>
     <t>81.157,</t>
   </si>
   <si>
@@ -340,9 +361,6 @@
     <t>0.000,</t>
   </si>
   <si>
-    <t>VectorX</t>
-  </si>
-  <si>
     <t>-1351.566,</t>
   </si>
   <si>
@@ -596,24 +614,6 @@
   </si>
   <si>
     <t>Width</t>
-  </si>
-  <si>
-    <t>EndPointx</t>
-  </si>
-  <si>
-    <t>EndPointy</t>
-  </si>
-  <si>
-    <t>EndPointz</t>
-  </si>
-  <si>
-    <t>StartPointz</t>
-  </si>
-  <si>
-    <t>StartPointy</t>
-  </si>
-  <si>
-    <t>StartPointx</t>
   </si>
 </sst>
 </file>
@@ -964,69 +964,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9301813B-72A7-4889-B3ED-651EE84C15A4}">
-  <dimension ref="A1:O106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618ACBDD-1880-436E-8556-D2B13A8B1992}">
+  <dimension ref="A1:R106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H1" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="I1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>189</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>188</v>
+        <v>28</v>
       </c>
       <c r="M1" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="N1" t="s">
-        <v>186</v>
+        <v>27</v>
       </c>
       <c r="O1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D2">
         <v>1441841</v>
@@ -1064,16 +1073,25 @@
       <c r="O2">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>-0.06</v>
+      </c>
+      <c r="Q2">
+        <v>-0.998</v>
+      </c>
+      <c r="R2">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>1441842</v>
@@ -1111,16 +1129,25 @@
       <c r="O3">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>0.06</v>
+      </c>
+      <c r="Q3">
+        <v>0.998</v>
+      </c>
+      <c r="R3">
+        <v>1354.002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D4">
         <v>1441843</v>
@@ -1158,16 +1185,25 @@
       <c r="O4">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>0.06</v>
+      </c>
+      <c r="Q4">
+        <v>0.998</v>
+      </c>
+      <c r="R4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>1441846</v>
@@ -1205,16 +1241,25 @@
       <c r="O5">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>0.998</v>
+      </c>
+      <c r="Q5">
+        <v>-0.06</v>
+      </c>
+      <c r="R5">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <v>1441847</v>
@@ -1252,16 +1297,25 @@
       <c r="O6">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>-0.998</v>
+      </c>
+      <c r="Q6">
+        <v>0.06</v>
+      </c>
+      <c r="R6">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>1441848</v>
@@ -1299,16 +1353,25 @@
       <c r="O7">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>-0.998</v>
+      </c>
+      <c r="Q7">
+        <v>0.06</v>
+      </c>
+      <c r="R7">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>1445057</v>
@@ -1346,16 +1409,25 @@
       <c r="O8">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>0.998</v>
+      </c>
+      <c r="Q8">
+        <v>-0.06</v>
+      </c>
+      <c r="R8">
+        <v>235.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <v>1445058</v>
@@ -1393,16 +1465,25 @@
       <c r="O9">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>0.06</v>
+      </c>
+      <c r="Q9">
+        <v>0.998</v>
+      </c>
+      <c r="R9">
+        <v>37.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <v>1445059</v>
@@ -1440,16 +1521,25 @@
       <c r="O10">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>-0.06</v>
+      </c>
+      <c r="Q10">
+        <v>-0.998</v>
+      </c>
+      <c r="R10">
+        <v>37.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D11">
         <v>1445060</v>
@@ -1487,16 +1577,25 @@
       <c r="O11">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>0.998</v>
+      </c>
+      <c r="Q11">
+        <v>-0.06</v>
+      </c>
+      <c r="R11">
+        <v>645.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <v>1476402</v>
@@ -1534,16 +1633,25 @@
       <c r="O12">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>0.998</v>
+      </c>
+      <c r="Q12">
+        <v>-0.06</v>
+      </c>
+      <c r="R12">
+        <v>235.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>1476459</v>
@@ -1581,16 +1689,25 @@
       <c r="O13">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>0.998</v>
+      </c>
+      <c r="Q13">
+        <v>-0.06</v>
+      </c>
+      <c r="R13">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>2347356</v>
@@ -1628,16 +1745,25 @@
       <c r="O14">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>0.06</v>
+      </c>
+      <c r="Q14">
+        <v>0.998</v>
+      </c>
+      <c r="R14">
+        <v>456.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>2347799</v>
@@ -1675,16 +1801,25 @@
       <c r="O15">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>-0.06</v>
+      </c>
+      <c r="Q15">
+        <v>-0.998</v>
+      </c>
+      <c r="R15">
+        <v>379.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D16">
         <v>2373268</v>
@@ -1722,16 +1857,25 @@
       <c r="O16">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>-0.998</v>
+      </c>
+      <c r="Q16">
+        <v>0.06</v>
+      </c>
+      <c r="R16">
+        <v>232.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D17">
         <v>2376175</v>
@@ -1769,16 +1913,25 @@
       <c r="O17">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>-0.06</v>
+      </c>
+      <c r="Q17">
+        <v>-0.998</v>
+      </c>
+      <c r="R17">
+        <v>256.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>2388008</v>
@@ -1816,16 +1969,25 @@
       <c r="O18">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>-0.998</v>
+      </c>
+      <c r="Q18">
+        <v>0.06</v>
+      </c>
+      <c r="R18">
+        <v>504.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>2477464</v>
@@ -1863,16 +2025,25 @@
       <c r="O19">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>-0.06</v>
+      </c>
+      <c r="Q19">
+        <v>-0.998</v>
+      </c>
+      <c r="R19">
+        <v>340.96499999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>2477467</v>
@@ -1910,16 +2081,25 @@
       <c r="O20">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>0.06</v>
+      </c>
+      <c r="Q20">
+        <v>0.998</v>
+      </c>
+      <c r="R20">
+        <v>355.57100000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D21">
         <v>2477468</v>
@@ -1957,16 +2137,25 @@
       <c r="O21">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>-0.998</v>
+      </c>
+      <c r="Q21">
+        <v>0.06</v>
+      </c>
+      <c r="R21">
+        <v>213.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D22">
         <v>2477844</v>
@@ -2004,16 +2193,25 @@
       <c r="O22">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>-0.06</v>
+      </c>
+      <c r="Q22">
+        <v>-0.998</v>
+      </c>
+      <c r="R22">
+        <v>634.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D23">
         <v>2479044</v>
@@ -2051,16 +2249,25 @@
       <c r="O23">
         <v>360</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>0.06</v>
+      </c>
+      <c r="Q23">
+        <v>0.998</v>
+      </c>
+      <c r="R23">
+        <v>203.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D24">
         <v>2493782</v>
@@ -2098,16 +2305,25 @@
       <c r="O24">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>-0.06</v>
+      </c>
+      <c r="Q24">
+        <v>-0.998</v>
+      </c>
+      <c r="R24">
+        <v>206.251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D25">
         <v>2493924</v>
@@ -2145,16 +2361,25 @@
       <c r="O25">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <v>-0.998</v>
+      </c>
+      <c r="Q25">
+        <v>0.06</v>
+      </c>
+      <c r="R25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D26">
         <v>2573915</v>
@@ -2192,16 +2417,25 @@
       <c r="O26">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>-0.06</v>
+      </c>
+      <c r="Q26">
+        <v>-0.998</v>
+      </c>
+      <c r="R26">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D27">
         <v>2586684</v>
@@ -2239,16 +2473,25 @@
       <c r="O27">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>-0.06</v>
+      </c>
+      <c r="Q27">
+        <v>-0.998</v>
+      </c>
+      <c r="R27">
+        <v>241.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D28">
         <v>2657732</v>
@@ -2286,16 +2529,25 @@
       <c r="O28">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28">
+        <v>0.06</v>
+      </c>
+      <c r="Q28">
+        <v>0.998</v>
+      </c>
+      <c r="R28">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D29">
         <v>2662918</v>
@@ -2333,16 +2585,25 @@
       <c r="O29">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>-0.06</v>
+      </c>
+      <c r="Q29">
+        <v>-0.998</v>
+      </c>
+      <c r="R29">
+        <v>355.572</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D30">
         <v>2662925</v>
@@ -2380,16 +2641,25 @@
       <c r="O30">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>-0.998</v>
+      </c>
+      <c r="Q30">
+        <v>0.06</v>
+      </c>
+      <c r="R30">
+        <v>36.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D31">
         <v>2662928</v>
@@ -2427,16 +2697,25 @@
       <c r="O31">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>0.06</v>
+      </c>
+      <c r="Q31">
+        <v>0.998</v>
+      </c>
+      <c r="R31">
+        <v>253.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D32">
         <v>2662992</v>
@@ -2474,16 +2753,25 @@
       <c r="O32">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>0.06</v>
+      </c>
+      <c r="Q32">
+        <v>0.998</v>
+      </c>
+      <c r="R32">
+        <v>634.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D33">
         <v>2663078</v>
@@ -2521,16 +2809,25 @@
       <c r="O33">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33">
+        <v>0.06</v>
+      </c>
+      <c r="Q33">
+        <v>0.998</v>
+      </c>
+      <c r="R33">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D34">
         <v>2668701</v>
@@ -2568,16 +2865,25 @@
       <c r="O34">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>-0.998</v>
+      </c>
+      <c r="Q34">
+        <v>0.06</v>
+      </c>
+      <c r="R34">
+        <v>504.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D35">
         <v>2671315</v>
@@ -2615,16 +2921,25 @@
       <c r="O35">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <v>-0.998</v>
+      </c>
+      <c r="Q35">
+        <v>0.06</v>
+      </c>
+      <c r="R35">
+        <v>681.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D36">
         <v>2673098</v>
@@ -2662,16 +2977,25 @@
       <c r="O36">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <v>-0.06</v>
+      </c>
+      <c r="Q36">
+        <v>-0.998</v>
+      </c>
+      <c r="R36">
+        <v>456.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D37">
         <v>2673099</v>
@@ -2709,16 +3033,25 @@
       <c r="O37">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <v>-0.06</v>
+      </c>
+      <c r="Q37">
+        <v>-0.998</v>
+      </c>
+      <c r="R37">
+        <v>360.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D38">
         <v>2673104</v>
@@ -2756,16 +3089,25 @@
       <c r="O38">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <v>-0.998</v>
+      </c>
+      <c r="Q38">
+        <v>0.06</v>
+      </c>
+      <c r="R38">
+        <v>217.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D39">
         <v>2673112</v>
@@ -2803,16 +3145,25 @@
       <c r="O39">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39">
+        <v>0.06</v>
+      </c>
+      <c r="Q39">
+        <v>0.998</v>
+      </c>
+      <c r="R39">
+        <v>545.47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D40">
         <v>2673113</v>
@@ -2850,16 +3201,25 @@
       <c r="O40">
         <v>58</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <v>-0.998</v>
+      </c>
+      <c r="Q40">
+        <v>0.06</v>
+      </c>
+      <c r="R40">
+        <v>217.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D41">
         <v>2673119</v>
@@ -2897,16 +3257,25 @@
       <c r="O41">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41">
+        <v>-0.998</v>
+      </c>
+      <c r="Q41">
+        <v>0.06</v>
+      </c>
+      <c r="R41">
+        <v>284.45999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D42">
         <v>2677885</v>
@@ -2944,16 +3313,25 @@
       <c r="O42">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>-0.06</v>
+      </c>
+      <c r="Q42">
+        <v>-0.998</v>
+      </c>
+      <c r="R42">
+        <v>390.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D43">
         <v>2679314</v>
@@ -2991,16 +3369,25 @@
       <c r="O43">
         <v>58</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <v>-0.06</v>
+      </c>
+      <c r="Q43">
+        <v>-0.998</v>
+      </c>
+      <c r="R43">
+        <v>409.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D44">
         <v>2734751</v>
@@ -3038,16 +3425,25 @@
       <c r="O44">
         <v>58</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P44">
+        <v>-0.06</v>
+      </c>
+      <c r="Q44">
+        <v>-0.998</v>
+      </c>
+      <c r="R44">
+        <v>456.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D45">
         <v>2734752</v>
@@ -3085,16 +3481,25 @@
       <c r="O45">
         <v>58</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P45">
+        <v>0.06</v>
+      </c>
+      <c r="Q45">
+        <v>0.998</v>
+      </c>
+      <c r="R45">
+        <v>379.74799999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D46">
         <v>2734755</v>
@@ -3132,16 +3537,25 @@
       <c r="O46">
         <v>58</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <v>-0.998</v>
+      </c>
+      <c r="Q46">
+        <v>0.06</v>
+      </c>
+      <c r="R46">
+        <v>232.499</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D47">
         <v>2734757</v>
@@ -3179,16 +3593,25 @@
       <c r="O47">
         <v>58</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P47">
+        <v>0.06</v>
+      </c>
+      <c r="Q47">
+        <v>0.998</v>
+      </c>
+      <c r="R47">
+        <v>256.49799999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D48">
         <v>2734760</v>
@@ -3226,16 +3649,25 @@
       <c r="O48">
         <v>58</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P48">
+        <v>-0.998</v>
+      </c>
+      <c r="Q48">
+        <v>0.06</v>
+      </c>
+      <c r="R48">
+        <v>496.24900000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D49">
         <v>2734763</v>
@@ -3273,16 +3705,25 @@
       <c r="O49">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49">
+        <v>0.06</v>
+      </c>
+      <c r="Q49">
+        <v>0.998</v>
+      </c>
+      <c r="R49">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D50">
         <v>2734771</v>
@@ -3320,16 +3761,25 @@
       <c r="O50">
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P50">
+        <v>-0.998</v>
+      </c>
+      <c r="Q50">
+        <v>0.06</v>
+      </c>
+      <c r="R50">
+        <v>496.24900000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D51">
         <v>2734777</v>
@@ -3367,16 +3817,25 @@
       <c r="O51">
         <v>58</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P51">
+        <v>-0.998</v>
+      </c>
+      <c r="Q51">
+        <v>0.06</v>
+      </c>
+      <c r="R51">
+        <v>673.25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D52">
         <v>2735641</v>
@@ -3414,16 +3873,25 @@
       <c r="O52">
         <v>58</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P52">
+        <v>0.06</v>
+      </c>
+      <c r="Q52">
+        <v>0.998</v>
+      </c>
+      <c r="R52">
+        <v>456.25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C53" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D53">
         <v>2735642</v>
@@ -3461,16 +3929,25 @@
       <c r="O53">
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P53">
+        <v>0.06</v>
+      </c>
+      <c r="Q53">
+        <v>0.998</v>
+      </c>
+      <c r="R53">
+        <v>379.74799999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D54">
         <v>2735646</v>
@@ -3508,16 +3985,25 @@
       <c r="O54">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P54">
+        <v>-0.998</v>
+      </c>
+      <c r="Q54">
+        <v>0.06</v>
+      </c>
+      <c r="R54">
+        <v>232.46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C55" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D55">
         <v>2735648</v>
@@ -3555,16 +4041,25 @@
       <c r="O55">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P55">
+        <v>-0.06</v>
+      </c>
+      <c r="Q55">
+        <v>-0.998</v>
+      </c>
+      <c r="R55">
+        <v>256.49799999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D56">
         <v>2735651</v>
@@ -3602,16 +4097,25 @@
       <c r="O56">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P56">
+        <v>-0.998</v>
+      </c>
+      <c r="Q56">
+        <v>0.06</v>
+      </c>
+      <c r="R56">
+        <v>521.21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D57">
         <v>2735654</v>
@@ -3649,16 +4153,25 @@
       <c r="O57">
         <v>58</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P57">
+        <v>-0.06</v>
+      </c>
+      <c r="Q57">
+        <v>-0.998</v>
+      </c>
+      <c r="R57">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D58">
         <v>2735655</v>
@@ -3696,16 +4209,25 @@
       <c r="O58">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P58">
+        <v>-0.998</v>
+      </c>
+      <c r="Q58">
+        <v>0.06</v>
+      </c>
+      <c r="R58">
+        <v>521.21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D59">
         <v>2735660</v>
@@ -3743,16 +4265,25 @@
       <c r="O59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P59">
+        <v>-0.998</v>
+      </c>
+      <c r="Q59">
+        <v>0.06</v>
+      </c>
+      <c r="R59">
+        <v>409.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D60">
         <v>2749243</v>
@@ -3790,16 +4321,25 @@
       <c r="O60">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P60">
+        <v>0.06</v>
+      </c>
+      <c r="Q60">
+        <v>0.998</v>
+      </c>
+      <c r="R60">
+        <v>193.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D61">
         <v>2749408</v>
@@ -3837,16 +4377,25 @@
       <c r="O61">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P61">
+        <v>-0.998</v>
+      </c>
+      <c r="Q61">
+        <v>0.06</v>
+      </c>
+      <c r="R61">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C62" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D62">
         <v>2756642</v>
@@ -3884,16 +4433,25 @@
       <c r="O62">
         <v>58</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P62">
+        <v>0.06</v>
+      </c>
+      <c r="Q62">
+        <v>0.998</v>
+      </c>
+      <c r="R62">
+        <v>191.499</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D63">
         <v>2756643</v>
@@ -3931,16 +4489,25 @@
       <c r="O63">
         <v>58</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P63">
+        <v>-0.06</v>
+      </c>
+      <c r="Q63">
+        <v>-0.998</v>
+      </c>
+      <c r="R63">
+        <v>191.499</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D64">
         <v>2756644</v>
@@ -3978,16 +4545,25 @@
       <c r="O64">
         <v>58</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P64">
+        <v>-0.998</v>
+      </c>
+      <c r="Q64">
+        <v>0.06</v>
+      </c>
+      <c r="R64">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C65" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D65">
         <v>2758691</v>
@@ -4025,16 +4601,25 @@
       <c r="O65">
         <v>360</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P65">
+        <v>0.06</v>
+      </c>
+      <c r="Q65">
+        <v>0.998</v>
+      </c>
+      <c r="R65">
+        <v>203.749</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D66">
         <v>2791656</v>
@@ -4072,16 +4657,25 @@
       <c r="O66">
         <v>58</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P66">
+        <v>-0.06</v>
+      </c>
+      <c r="Q66">
+        <v>-0.998</v>
+      </c>
+      <c r="R66">
+        <v>37.752000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D67">
         <v>2816671</v>
@@ -4119,16 +4713,25 @@
       <c r="O67">
         <v>58</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P67">
+        <v>0.998</v>
+      </c>
+      <c r="Q67">
+        <v>-0.06</v>
+      </c>
+      <c r="R67">
+        <v>675.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C68" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D68">
         <v>2817053</v>
@@ -4166,16 +4769,25 @@
       <c r="O68">
         <v>58</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P68">
+        <v>0.06</v>
+      </c>
+      <c r="Q68">
+        <v>0.998</v>
+      </c>
+      <c r="R68">
+        <v>37.752000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C69" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D69">
         <v>2865100</v>
@@ -4213,16 +4825,25 @@
       <c r="O69">
         <v>58</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P69">
+        <v>-0.998</v>
+      </c>
+      <c r="Q69">
+        <v>0.06</v>
+      </c>
+      <c r="R69">
+        <v>201.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C70" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D70">
         <v>2981356</v>
@@ -4260,16 +4881,25 @@
       <c r="O70">
         <v>58</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P70">
+        <v>0.06</v>
+      </c>
+      <c r="Q70">
+        <v>0.998</v>
+      </c>
+      <c r="R70">
+        <v>123.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C71" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D71">
         <v>2984283</v>
@@ -4307,16 +4937,25 @@
       <c r="O71">
         <v>58</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P71">
+        <v>-0.998</v>
+      </c>
+      <c r="Q71">
+        <v>0.06</v>
+      </c>
+      <c r="R71">
+        <v>413.79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D72">
         <v>3009845</v>
@@ -4354,16 +4993,25 @@
       <c r="O72">
         <v>58</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P72">
+        <v>-0.998</v>
+      </c>
+      <c r="Q72">
+        <v>0.06</v>
+      </c>
+      <c r="R72">
+        <v>288.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B73" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C73" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D73">
         <v>3118291</v>
@@ -4401,16 +5049,25 @@
       <c r="O73">
         <v>58</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P73">
+        <v>0.06</v>
+      </c>
+      <c r="Q73">
+        <v>0.998</v>
+      </c>
+      <c r="R73">
+        <v>390.255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D74">
         <v>3118293</v>
@@ -4448,16 +5105,25 @@
       <c r="O74">
         <v>58</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P74">
+        <v>0.06</v>
+      </c>
+      <c r="Q74">
+        <v>0.998</v>
+      </c>
+      <c r="R74">
+        <v>390.255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C75" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D75">
         <v>3199261</v>
@@ -4495,16 +5161,25 @@
       <c r="O75">
         <v>58</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P75">
+        <v>-0.06</v>
+      </c>
+      <c r="Q75">
+        <v>-0.998</v>
+      </c>
+      <c r="R75">
+        <v>250.00299999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D76">
         <v>3231003</v>
@@ -4542,16 +5217,25 @@
       <c r="O76">
         <v>58</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P76">
+        <v>-0.998</v>
+      </c>
+      <c r="Q76">
+        <v>0.06</v>
+      </c>
+      <c r="R76">
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C77" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D77">
         <v>3231005</v>
@@ -4589,16 +5273,25 @@
       <c r="O77">
         <v>58</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P77">
+        <v>-0.06</v>
+      </c>
+      <c r="Q77">
+        <v>-0.998</v>
+      </c>
+      <c r="R77">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C78" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D78">
         <v>3231779</v>
@@ -4636,16 +5329,25 @@
       <c r="O78">
         <v>58</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P78">
+        <v>-0.06</v>
+      </c>
+      <c r="Q78">
+        <v>-0.998</v>
+      </c>
+      <c r="R78">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="C79" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D79">
         <v>3244379</v>
@@ -4683,16 +5385,25 @@
       <c r="O79">
         <v>58</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P79">
+        <v>-0.998</v>
+      </c>
+      <c r="Q79">
+        <v>0.06</v>
+      </c>
+      <c r="R79">
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C80" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D80">
         <v>3244384</v>
@@ -4730,16 +5441,25 @@
       <c r="O80">
         <v>58</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P80">
+        <v>0.06</v>
+      </c>
+      <c r="Q80">
+        <v>0.998</v>
+      </c>
+      <c r="R80">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C81" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D81">
         <v>3244385</v>
@@ -4777,16 +5497,25 @@
       <c r="O81">
         <v>58</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P81">
+        <v>0.06</v>
+      </c>
+      <c r="Q81">
+        <v>0.998</v>
+      </c>
+      <c r="R81">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B82" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D82">
         <v>3314422</v>
@@ -4824,16 +5553,25 @@
       <c r="O82">
         <v>58</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P82">
+        <v>-0.06</v>
+      </c>
+      <c r="Q82">
+        <v>-0.998</v>
+      </c>
+      <c r="R82">
+        <v>123.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C83" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D83">
         <v>3324300</v>
@@ -4871,16 +5609,25 @@
       <c r="O83">
         <v>58</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P83">
+        <v>0.998</v>
+      </c>
+      <c r="Q83">
+        <v>-0.06</v>
+      </c>
+      <c r="R83">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B84" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C84" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D84">
         <v>3324305</v>
@@ -4918,16 +5665,25 @@
       <c r="O84">
         <v>58</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P84">
+        <v>-0.998</v>
+      </c>
+      <c r="Q84">
+        <v>0.06</v>
+      </c>
+      <c r="R84">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B85" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C85" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D85">
         <v>3324306</v>
@@ -4965,16 +5721,25 @@
       <c r="O85">
         <v>58</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P85">
+        <v>-0.06</v>
+      </c>
+      <c r="Q85">
+        <v>-0.998</v>
+      </c>
+      <c r="R85">
+        <v>138.035</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B86" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C86" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D86">
         <v>3325570</v>
@@ -5012,16 +5777,25 @@
       <c r="O86">
         <v>58</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P86">
+        <v>0.998</v>
+      </c>
+      <c r="Q86">
+        <v>-0.06</v>
+      </c>
+      <c r="R86">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B87" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C87" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D87">
         <v>3325571</v>
@@ -5059,16 +5833,25 @@
       <c r="O87">
         <v>58</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P87">
+        <v>-0.06</v>
+      </c>
+      <c r="Q87">
+        <v>-0.998</v>
+      </c>
+      <c r="R87">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C88" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D88">
         <v>3325573</v>
@@ -5106,16 +5889,25 @@
       <c r="O88">
         <v>58</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P88">
+        <v>0.06</v>
+      </c>
+      <c r="Q88">
+        <v>0.998</v>
+      </c>
+      <c r="R88">
+        <v>129.20599999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B89" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C89" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D89">
         <v>3325874</v>
@@ -5153,16 +5945,25 @@
       <c r="O89">
         <v>58</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P89">
+        <v>0.998</v>
+      </c>
+      <c r="Q89">
+        <v>-0.06</v>
+      </c>
+      <c r="R89">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C90" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D90">
         <v>3325875</v>
@@ -5200,16 +6001,25 @@
       <c r="O90">
         <v>58</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P90">
+        <v>0.06</v>
+      </c>
+      <c r="Q90">
+        <v>0.998</v>
+      </c>
+      <c r="R90">
+        <v>90.765000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B91" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C91" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D91">
         <v>3325876</v>
@@ -5247,16 +6057,25 @@
       <c r="O91">
         <v>58</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P91">
+        <v>-0.998</v>
+      </c>
+      <c r="Q91">
+        <v>0.06</v>
+      </c>
+      <c r="R91">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B92" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C92" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D92">
         <v>3325877</v>
@@ -5294,16 +6113,25 @@
       <c r="O92">
         <v>58</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P92">
+        <v>-0.06</v>
+      </c>
+      <c r="Q92">
+        <v>-0.998</v>
+      </c>
+      <c r="R92">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C93" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D93">
         <v>3337863</v>
@@ -5341,16 +6169,25 @@
       <c r="O93">
         <v>58</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P93">
+        <v>0.06</v>
+      </c>
+      <c r="Q93">
+        <v>0.998</v>
+      </c>
+      <c r="R93">
+        <v>123.25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B94" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C94" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D94">
         <v>3338520</v>
@@ -5388,16 +6225,25 @@
       <c r="O94">
         <v>58</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P94">
+        <v>-0.06</v>
+      </c>
+      <c r="Q94">
+        <v>-0.998</v>
+      </c>
+      <c r="R94">
+        <v>123.25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C95" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D95">
         <v>3354733</v>
@@ -5435,16 +6281,25 @@
       <c r="O95">
         <v>58</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P95">
+        <v>-0.998</v>
+      </c>
+      <c r="Q95">
+        <v>0.06</v>
+      </c>
+      <c r="R95">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D96">
         <v>3365155</v>
@@ -5482,16 +6337,25 @@
       <c r="O96">
         <v>58</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P96">
+        <v>0.998</v>
+      </c>
+      <c r="Q96">
+        <v>-0.06</v>
+      </c>
+      <c r="R96">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C97" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D97">
         <v>3365156</v>
@@ -5529,16 +6393,25 @@
       <c r="O97">
         <v>58</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P97">
+        <v>0.06</v>
+      </c>
+      <c r="Q97">
+        <v>0.998</v>
+      </c>
+      <c r="R97">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C98" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D98">
         <v>3365157</v>
@@ -5576,16 +6449,25 @@
       <c r="O98">
         <v>58</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P98">
+        <v>-0.998</v>
+      </c>
+      <c r="Q98">
+        <v>0.06</v>
+      </c>
+      <c r="R98">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B99" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C99" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D99">
         <v>3471180</v>
@@ -5623,16 +6505,25 @@
       <c r="O99">
         <v>58</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P99">
+        <v>0.998</v>
+      </c>
+      <c r="Q99">
+        <v>-0.06</v>
+      </c>
+      <c r="R99">
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B100" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C100" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D100">
         <v>3471329</v>
@@ -5670,16 +6561,25 @@
       <c r="O100">
         <v>58</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P100">
+        <v>-0.998</v>
+      </c>
+      <c r="Q100">
+        <v>0.06</v>
+      </c>
+      <c r="R100">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B101" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D101">
         <v>3471462</v>
@@ -5717,16 +6617,25 @@
       <c r="O101">
         <v>58</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P101">
+        <v>0.998</v>
+      </c>
+      <c r="Q101">
+        <v>-0.06</v>
+      </c>
+      <c r="R101">
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B102" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C102" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D102">
         <v>3471463</v>
@@ -5764,16 +6673,25 @@
       <c r="O102">
         <v>58</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P102">
+        <v>-0.998</v>
+      </c>
+      <c r="Q102">
+        <v>0.06</v>
+      </c>
+      <c r="R102">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B103" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C103" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D103">
         <v>3924178</v>
@@ -5811,16 +6729,25 @@
       <c r="O103">
         <v>58</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P103">
+        <v>-0.998</v>
+      </c>
+      <c r="Q103">
+        <v>0.06</v>
+      </c>
+      <c r="R103">
+        <v>288.75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B104" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C104" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D104">
         <v>3925910</v>
@@ -5858,16 +6785,25 @@
       <c r="O104">
         <v>58</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P104">
+        <v>-0.998</v>
+      </c>
+      <c r="Q104">
+        <v>0.06</v>
+      </c>
+      <c r="R104">
+        <v>506.25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B105" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C105" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D105">
         <v>4033220</v>
@@ -5905,16 +6841,25 @@
       <c r="O105">
         <v>58</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P105">
+        <v>-0.998</v>
+      </c>
+      <c r="Q105">
+        <v>0.06</v>
+      </c>
+      <c r="R105">
+        <v>201.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="B106" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C106" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D106">
         <v>4200547</v>
@@ -5951,6 +6896,15 @@
       </c>
       <c r="O106">
         <v>0</v>
+      </c>
+      <c r="P106">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="Q106">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="R106">
+        <v>2382.5</v>
       </c>
     </row>
   </sheetData>
@@ -5959,7 +6913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0B3E26-3784-4340-8158-51EB5914F440}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6410AFB6-5A57-48AA-A3B3-F620C95FD86E}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6275,7 +7229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C00C80-34AF-48B9-BD36-B0F7E0EDC3EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70FA89D-9B64-471C-9BF8-AF05D1F1EFB3}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6475,7 +7429,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599C07D6-AE3C-4324-B454-1E150FE01E06}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B2DA84-8F03-4290-ACAC-6EB43A68E122}">
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7160,7 +8114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6120E7-3344-41F9-9DAA-53C7A72DE5E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC966EDB-44DB-45BB-8A5C-0DF98E53B087}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7313,7 +8267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7AA741-ACA8-4B39-A13A-138ABA76360D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8DBF8A-B6C0-4697-BF87-81D3194CF629}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>